<commit_message>
Add get user by id and some compact in echo_bot
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -332,10 +332,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -370,7 +370,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>12332</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="3">
@@ -403,7 +403,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>12332</v>
+        <v>1231532</v>
       </c>
     </row>
     <row r="8">
@@ -436,7 +436,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>12332</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13">
@@ -469,7 +469,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>12332</v>
+        <v>2</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -494,7 +494,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>12332</v>
+        <v>33</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -519,7 +519,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>12332</v>
+        <v>333</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -567,9 +567,34 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1578</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Pidor</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>['Web','SCSS','DevOps']</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>['Web','SCSS','DevOps']</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>['Web','SCSS','DevOps']</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.7007874015748032" right="0.7007874015748032" top="0.7519685039370079" bottom="0.7519685039370079" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="4294967295" useFirstPageNumber="0" pageOrder="downThenOver" usePrinterDefaults="1" blackAndWhite="0" draft="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="2147483648" useFirstPageNumber="0" pageOrder="downThenOver" usePrinterDefaults="1" blackAndWhite="0" draft="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
 </worksheet>
 </file>
</xml_diff>